<commit_message>
fully working script. in the middle of implementing cmd argument
</commit_message>
<xml_diff>
--- a/Tata Sky Channels List.xlsx
+++ b/Tata Sky Channels List.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="80">
   <si>
     <t xml:space="preserve">Channel Number</t>
   </si>
@@ -46,7 +46,7 @@
     <t xml:space="preserve">DD National</t>
   </si>
   <si>
-    <t xml:space="preserve">Lok Sabha TV</t>
+    <t xml:space="preserve">Lok Sabha</t>
   </si>
   <si>
     <t xml:space="preserve">Rajya Sabha</t>
@@ -64,10 +64,10 @@
     <t xml:space="preserve">9XM</t>
   </si>
   <si>
-    <t xml:space="preserve">Z News</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Z Business</t>
+    <t xml:space="preserve">Zee News</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zee Business</t>
   </si>
   <si>
     <t xml:space="preserve">#Z Cinema HD</t>
@@ -79,16 +79,16 @@
     <t xml:space="preserve">#&amp; pictures HD</t>
   </si>
   <si>
-    <t xml:space="preserve">FOX Life HD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Movies OK </t>
+    <t xml:space="preserve">Fox Life HD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Movies Ok</t>
   </si>
   <si>
     <t xml:space="preserve">Nat Geo People HD</t>
   </si>
   <si>
-    <t xml:space="preserve">Nat Geo HD</t>
+    <t xml:space="preserve">National Geographic HD</t>
   </si>
   <si>
     <t xml:space="preserve">#Sony MAX HD</t>
@@ -97,13 +97,13 @@
     <t xml:space="preserve">#20.06</t>
   </si>
   <si>
-    <t xml:space="preserve">Sony MIX</t>
+    <t xml:space="preserve">Sony Mix</t>
   </si>
   <si>
     <t xml:space="preserve">SET HD</t>
   </si>
   <si>
-    <t xml:space="preserve">Sony MAX 2</t>
+    <t xml:space="preserve">Sony Max 2</t>
   </si>
   <si>
     <t xml:space="preserve">CNBC TV18</t>
@@ -112,13 +112,13 @@
     <t xml:space="preserve">CNBC TV18 Prime HD</t>
   </si>
   <si>
-    <t xml:space="preserve">CNN News 18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CNBC Awaaz </t>
-  </si>
-  <si>
-    <t xml:space="preserve">FYI TV 18</t>
+    <t xml:space="preserve">CNN News18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CNBC Awaaz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FYI TV18</t>
   </si>
   <si>
     <t xml:space="preserve">History TV18 HD</t>
@@ -130,7 +130,7 @@
     <t xml:space="preserve">MTV Beats HD</t>
   </si>
   <si>
-    <t xml:space="preserve">VH1 HD</t>
+    <t xml:space="preserve">Vh1 HD</t>
   </si>
   <si>
     <t xml:space="preserve">UTV HD</t>
@@ -148,7 +148,7 @@
     <t xml:space="preserve">WB</t>
   </si>
   <si>
-    <t xml:space="preserve">MN+HD</t>
+    <t xml:space="preserve">MN+ HD</t>
   </si>
   <si>
     <t xml:space="preserve">Movies Now HD</t>
@@ -260,9 +260,6 @@
   </si>
   <si>
     <t xml:space="preserve">News Nation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total</t>
   </si>
 </sst>
 </file>
@@ -389,8 +386,8 @@
   </sheetPr>
   <dimension ref="A1:E75"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A35" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B36" activeCellId="0" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1031,9 +1028,7 @@
       </c>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B75" s="1" t="s">
-        <v>80</v>
-      </c>
+      <c r="B75" s="1"/>
       <c r="C75" s="1" t="n">
         <f aca="false">SUM(C2:C73)</f>
         <v>150.16</v>

</xml_diff>